<commit_message>
Added email, SoundCloud, Goodreads
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28340" yWindow="8560" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Twitter</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>FF6600</t>
+  </si>
+  <si>
+    <t>Goodreads</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Soundcloud</t>
+  </si>
+  <si>
+    <t>5A471B</t>
   </si>
 </sst>
 </file>
@@ -694,11 +706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1129,28 +1141,28 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C21">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <f>MOD((C21+100),360)</f>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -1171,17 +1183,17 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <f>MOD((C23+100),360)</f>
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -1192,176 +1204,239 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C24">
-        <v>11.2</v>
+        <v>24</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>111.2</v>
+        <v>124</v>
       </c>
       <c r="E24">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F24">
-        <v>92.2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D25">
         <f>MOD((C25+100),360)</f>
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E25">
-        <v>74.2</v>
+        <v>100</v>
       </c>
       <c r="F25">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>11.2</v>
       </c>
       <c r="D26">
         <f>MOD((C26+100),360)</f>
-        <v>104</v>
+        <v>111.2</v>
       </c>
       <c r="E26">
-        <v>92.5</v>
+        <v>84.7</v>
       </c>
       <c r="F26">
-        <v>89.4</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D27">
         <f>MOD((C27+100),360)</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E27">
-        <v>97</v>
+        <v>74.2</v>
       </c>
       <c r="F27">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28">
-        <v>444444</v>
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <f>MOD((C28+100),360)</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>92.5</v>
       </c>
       <c r="F28">
-        <v>27</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C29">
-        <v>357.5</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <f>MOD((C29+100),360)</f>
-        <v>97.5</v>
+        <v>103</v>
       </c>
       <c r="E29">
-        <v>84.2</v>
+        <v>97</v>
       </c>
       <c r="F29">
-        <v>79.599999999999994</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>20</v>
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>444444</v>
       </c>
       <c r="C30">
-        <v>336.8</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>100</v>
       </c>
       <c r="E30">
-        <v>67.5</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>91.8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>666666</v>
       </c>
       <c r="C31">
-        <v>287.3</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>357.5</v>
+      </c>
+      <c r="D32">
+        <f>MOD((C32+100),360)</f>
+        <v>97.5</v>
+      </c>
+      <c r="E32">
+        <v>84.2</v>
+      </c>
+      <c r="F32">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>336.8</v>
+      </c>
+      <c r="D33">
+        <f>MOD((C33+100),360)</f>
+        <v>76.800000000000011</v>
+      </c>
+      <c r="E33">
+        <v>67.5</v>
+      </c>
+      <c r="F33">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>287.3</v>
+      </c>
+      <c r="D34">
+        <f>MOD((C34+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>81.3</v>
       </c>
-      <c r="F31">
+      <c r="F34">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F31">
-      <sortCondition descending="1" ref="D1:D31"/>
+    <sortState ref="A2:F34">
+      <sortCondition descending="1" ref="D1:D34"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Behance and Dropbox icons
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -168,9 +168,6 @@
     <t>Dropbox</t>
   </si>
   <si>
-    <t>2180CC</t>
-  </si>
-  <si>
     <t>1769FF</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>5A471B</t>
+  </si>
+  <si>
+    <t>2281CF</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -784,10 +784,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>219</v>
@@ -871,7 +871,7 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>207</v>
@@ -884,15 +884,15 @@
         <v>84</v>
       </c>
       <c r="F8">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>204</v>
@@ -952,10 +952,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
       </c>
       <c r="C12">
         <v>199</v>
@@ -973,10 +973,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13">
         <v>198</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>84</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>42</v>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
       </c>
       <c r="C24">
         <v>24</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>444444</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>666666</v>

</xml_diff>

<commit_message>
Updated to reflect new RSS colour
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Twitter</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>2281CF</t>
+  </si>
+  <si>
+    <t>FF8300</t>
   </si>
 </sst>
 </file>
@@ -710,7 +713,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1207,14 +1210,14 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C24">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E24">
         <v>100</v>

</xml_diff>

<commit_message>
Added About.me and Instagram
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="28060" yWindow="2120" windowWidth="11400" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Twitter</t>
   </si>
@@ -253,6 +253,24 @@
   </si>
   <si>
     <t>CD332D</t>
+  </si>
+  <si>
+    <t>About.me</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>00405D</t>
+  </si>
+  <si>
+    <t>3F729B</t>
+  </si>
+  <si>
+    <t>App.net</t>
+  </si>
+  <si>
+    <t>898D90</t>
   </si>
 </sst>
 </file>
@@ -733,11 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -916,335 +934,335 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C9">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D9">
         <f>MOD((C9+100),360)</f>
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E9">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C10">
-        <v>201.8</v>
+        <v>206</v>
       </c>
       <c r="D10">
         <f>MOD((C10+100),360)</f>
-        <v>301.8</v>
+        <v>306</v>
       </c>
       <c r="E10">
-        <v>73.3</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C11">
-        <v>199.8</v>
+        <v>204</v>
       </c>
       <c r="D11">
         <f>MOD((C11+100),360)</f>
-        <v>299.8</v>
+        <v>304</v>
       </c>
       <c r="E11">
-        <v>74.599999999999994</v>
+        <v>55</v>
       </c>
       <c r="F11">
-        <v>87.8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>199</v>
+        <v>201.8</v>
       </c>
       <c r="D12">
         <f>MOD((C12+100),360)</f>
-        <v>299</v>
+        <v>301.8</v>
       </c>
       <c r="E12">
-        <v>79</v>
+        <v>73.3</v>
       </c>
       <c r="F12">
-        <v>61</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>198</v>
+        <v>199.8</v>
       </c>
       <c r="D13">
         <f>MOD((C13+100),360)</f>
-        <v>298</v>
+        <v>299.8</v>
       </c>
       <c r="E13">
-        <v>83</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="F13">
-        <v>79</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C14">
-        <v>196.9</v>
+        <v>199</v>
       </c>
       <c r="D14">
         <f>MOD((C14+100),360)</f>
-        <v>296.89999999999998</v>
+        <v>299</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F14">
-        <v>69.400000000000006</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C15">
-        <v>196.3</v>
+        <v>199</v>
       </c>
       <c r="D15">
         <f>MOD((C15+100),360)</f>
-        <v>296.3</v>
+        <v>299</v>
       </c>
       <c r="E15">
         <v>100</v>
       </c>
       <c r="F15">
-        <v>94.1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C16">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D16">
         <f>MOD((C16+100),360)</f>
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E16">
-        <v>4.0999999999999996</v>
+        <v>83</v>
       </c>
       <c r="F16">
-        <v>75.7</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C17">
-        <v>84</v>
+        <v>196.9</v>
       </c>
       <c r="D17">
         <f>MOD((C17+100),360)</f>
-        <v>184</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="E17">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="F17">
-        <v>64</v>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C18">
-        <v>81</v>
+        <v>196.3</v>
       </c>
       <c r="D18">
         <f>MOD((C18+100),360)</f>
-        <v>181</v>
+        <v>296.3</v>
       </c>
       <c r="E18">
         <v>100</v>
       </c>
       <c r="F18">
-        <v>64</v>
+        <v>94.1</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>80.900000000000006</v>
+        <v>195</v>
       </c>
       <c r="D19">
         <f>MOD((C19+100),360)</f>
-        <v>180.9</v>
+        <v>295</v>
       </c>
       <c r="E19">
-        <v>86.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F19">
-        <v>71.8</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C20">
-        <v>74.5</v>
+        <v>84</v>
       </c>
       <c r="D20">
         <f>MOD((C20+100),360)</f>
-        <v>174.5</v>
+        <v>184</v>
       </c>
       <c r="E20">
-        <v>71.2</v>
+        <v>53</v>
       </c>
       <c r="F20">
-        <v>77.599999999999994</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C21">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D21">
         <f>MOD((C21+100),360)</f>
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="E21">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>42</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D22">
         <f>MOD((C22+100),360)</f>
-        <v>142</v>
+        <v>180.9</v>
       </c>
       <c r="E22">
-        <v>70</v>
+        <v>86.3</v>
       </c>
       <c r="F22">
-        <v>35</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C23">
-        <v>36</v>
+        <v>74.5</v>
       </c>
       <c r="D23">
         <f>MOD((C23+100),360)</f>
-        <v>136</v>
+        <v>174.5</v>
       </c>
       <c r="E23">
-        <v>100</v>
+        <v>71.2</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C24">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F24">
         <v>100</v>
@@ -1252,59 +1270,59 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <f>MOD((C25+100),360)</f>
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D26">
         <f>MOD((C26+100),360)</f>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E26">
         <v>100</v>
       </c>
       <c r="F26">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D27">
         <f>MOD((C27+100),360)</f>
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1315,239 +1333,302 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C28">
-        <v>11.2</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <f>MOD((C28+100),360)</f>
-        <v>111.2</v>
+        <v>131</v>
       </c>
       <c r="E28">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F28">
-        <v>92.2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D29">
         <f>MOD((C29+100),360)</f>
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E29">
-        <v>74.2</v>
+        <v>100</v>
       </c>
       <c r="F29">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="E30">
-        <v>92.5</v>
+        <v>100</v>
       </c>
       <c r="F30">
-        <v>89.4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>11.2</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
-        <v>103</v>
+        <v>111.2</v>
       </c>
       <c r="E31">
-        <v>97</v>
+        <v>84.7</v>
       </c>
       <c r="F31">
-        <v>84</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <f>MOD((C32+100),360)</f>
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E32">
-        <v>78</v>
+        <v>74.2</v>
       </c>
       <c r="F32">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33">
-        <v>444444</v>
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D33">
         <f>MOD((C33+100),360)</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>92.5</v>
       </c>
       <c r="F33">
-        <v>27</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34">
-        <v>666666</v>
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D34">
         <f>MOD((C34+100),360)</f>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="F34">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="C35">
-        <v>357.5</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <f>MOD((C35+100),360)</f>
-        <v>97.5</v>
+        <v>102</v>
       </c>
       <c r="E35">
-        <v>84.2</v>
+        <v>78</v>
       </c>
       <c r="F35">
-        <v>79.599999999999994</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <v>444444</v>
       </c>
       <c r="C36">
-        <v>336.8</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <f>MOD((C36+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>100</v>
       </c>
       <c r="E36">
-        <v>67.5</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>91.8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>666666</v>
       </c>
       <c r="C37">
-        <v>328</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <f>MOD((C37+100),360)</f>
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E37">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>93</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C38">
-        <v>287.3</v>
+        <v>357.5</v>
       </c>
       <c r="D38">
         <f>MOD((C38+100),360)</f>
+        <v>97.5</v>
+      </c>
+      <c r="E38">
+        <v>84.2</v>
+      </c>
+      <c r="F38">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>336.8</v>
+      </c>
+      <c r="D39">
+        <f>MOD((C39+100),360)</f>
+        <v>76.800000000000011</v>
+      </c>
+      <c r="E39">
+        <v>67.5</v>
+      </c>
+      <c r="F39">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40">
+        <v>328</v>
+      </c>
+      <c r="D40">
+        <f>MOD((C40+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E40">
+        <v>84</v>
+      </c>
+      <c r="F40">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>287.3</v>
+      </c>
+      <c r="D41">
+        <f>MOD((C41+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E38">
+      <c r="E41">
         <v>81.3</v>
       </c>
-      <c r="F38">
+      <c r="F41">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F38">
-      <sortCondition descending="1" ref="D1:D38"/>
+    <sortState ref="A2:F41">
+      <sortCondition descending="1" ref="D1:D41"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Evernote and Event Store
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28060" yWindow="2120" windowWidth="11400" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9020" windowHeight="18200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Twitter</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>898D90</t>
+  </si>
+  <si>
+    <t>Evernote</t>
+  </si>
+  <si>
+    <t>7AC142</t>
   </si>
 </sst>
 </file>
@@ -751,11 +757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1165,41 +1171,41 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C20">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="D20">
         <f>MOD((C20+100),360)</f>
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="E20">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="F20">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C21">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D21">
         <f>MOD((C21+100),360)</f>
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="F21">
         <v>64</v>
@@ -1207,112 +1213,112 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C22">
-        <v>80.900000000000006</v>
+        <v>81</v>
       </c>
       <c r="D22">
         <f>MOD((C22+100),360)</f>
-        <v>180.9</v>
+        <v>181</v>
       </c>
       <c r="E22">
-        <v>86.3</v>
+        <v>100</v>
       </c>
       <c r="F22">
-        <v>71.8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>74.5</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D23">
         <f>MOD((C23+100),360)</f>
-        <v>174.5</v>
+        <v>180.9</v>
       </c>
       <c r="E23">
-        <v>71.2</v>
+        <v>86.3</v>
       </c>
       <c r="F23">
-        <v>77.599999999999994</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C24">
-        <v>46</v>
+        <v>74.5</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>146</v>
+        <v>174.5</v>
       </c>
       <c r="E24">
-        <v>59</v>
+        <v>71.2</v>
       </c>
       <c r="F24">
-        <v>100</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C25">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <f>MOD((C25+100),360)</f>
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F25">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C26">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D26">
         <f>MOD((C26+100),360)</f>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -1333,17 +1339,17 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D28">
         <f>MOD((C28+100),360)</f>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E28">
         <v>100</v>
@@ -1354,10 +1360,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C29">
         <v>31</v>
@@ -1370,162 +1376,162 @@
         <v>100</v>
       </c>
       <c r="F29">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C30">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E30">
         <v>100</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C31">
-        <v>11.2</v>
+        <v>24</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
-        <v>111.2</v>
+        <v>124</v>
       </c>
       <c r="E31">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F31">
-        <v>92.2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>11.2</v>
       </c>
       <c r="D32">
         <f>MOD((C32+100),360)</f>
-        <v>107</v>
+        <v>111.2</v>
       </c>
       <c r="E32">
-        <v>74.2</v>
+        <v>84.7</v>
       </c>
       <c r="F32">
-        <v>82</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
         <v>7</v>
-      </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
       </c>
       <c r="D33">
         <f>MOD((C33+100),360)</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E33">
-        <v>92.5</v>
+        <v>74.2</v>
       </c>
       <c r="F33">
-        <v>89.4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34">
         <f>MOD((C34+100),360)</f>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34">
-        <v>97</v>
+        <v>92.5</v>
       </c>
       <c r="F34">
-        <v>84</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <f>MOD((C35+100),360)</f>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E35">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="F35">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36">
-        <v>444444</v>
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36">
         <f>MOD((C36+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F36">
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B37">
-        <v>666666</v>
+        <v>444444</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1538,97 +1544,118 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="B38">
+        <v>666666</v>
       </c>
       <c r="C38">
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>MOD((C38+100),360)</f>
-        <v>97.5</v>
+        <v>100</v>
       </c>
       <c r="E38">
-        <v>84.2</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>79.599999999999994</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C39">
-        <v>336.8</v>
+        <v>357.5</v>
       </c>
       <c r="D39">
         <f>MOD((C39+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>97.5</v>
       </c>
       <c r="E39">
-        <v>67.5</v>
+        <v>84.2</v>
       </c>
       <c r="F39">
-        <v>91.8</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C40">
-        <v>328</v>
+        <v>336.8</v>
       </c>
       <c r="D40">
         <f>MOD((C40+100),360)</f>
-        <v>68</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="E40">
-        <v>84</v>
+        <v>67.5</v>
       </c>
       <c r="F40">
-        <v>93</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="C41">
-        <v>287.3</v>
+        <v>328</v>
       </c>
       <c r="D41">
         <f>MOD((C41+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E41">
+        <v>84</v>
+      </c>
+      <c r="F41">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <v>287.3</v>
+      </c>
+      <c r="D42">
+        <f>MOD((C42+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>81.3</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F41">
-      <sortCondition descending="1" ref="D1:D41"/>
+    <sortState ref="A2:F42">
+      <sortCondition descending="1" ref="D1:D42"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Simple Icons icon
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9020" windowHeight="18200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16120" windowHeight="23380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>Twitter</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>7AC142</t>
+  </si>
+  <si>
+    <t>Simple Icons</t>
+  </si>
+  <si>
+    <t>BF1813</t>
   </si>
 </sst>
 </file>
@@ -757,11 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1528,31 +1534,31 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37">
-        <v>444444</v>
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <f>MOD((C37+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F37">
-        <v>27</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B38">
-        <v>666666</v>
+        <v>444444</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1565,97 +1571,118 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="B39">
+        <v>666666</v>
       </c>
       <c r="C39">
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <f>MOD((C39+100),360)</f>
-        <v>97.5</v>
+        <v>100</v>
       </c>
       <c r="E39">
-        <v>84.2</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>79.599999999999994</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C40">
-        <v>336.8</v>
+        <v>357.5</v>
       </c>
       <c r="D40">
         <f>MOD((C40+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>97.5</v>
       </c>
       <c r="E40">
-        <v>67.5</v>
+        <v>84.2</v>
       </c>
       <c r="F40">
-        <v>91.8</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>328</v>
+        <v>336.8</v>
       </c>
       <c r="D41">
         <f>MOD((C41+100),360)</f>
-        <v>68</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="E41">
-        <v>84</v>
+        <v>67.5</v>
       </c>
       <c r="F41">
-        <v>93</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="C42">
-        <v>287.3</v>
+        <v>328</v>
       </c>
       <c r="D42">
         <f>MOD((C42+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E42">
+        <v>84</v>
+      </c>
+      <c r="F42">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43">
+        <v>287.3</v>
+      </c>
+      <c r="D43">
+        <f>MOD((C43+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <v>81.3</v>
       </c>
-      <c r="F42">
+      <c r="F43">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F42">
-      <sortCondition descending="1" ref="D1:D42"/>
+    <sortState ref="A2:F43">
+      <sortCondition descending="1" ref="D1:D43"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Stack Exchange sites
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16120" windowHeight="23380" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>Twitter</t>
   </si>
@@ -283,6 +283,24 @@
   </si>
   <si>
     <t>BF1813</t>
+  </si>
+  <si>
+    <t>Super User</t>
+  </si>
+  <si>
+    <t>Stack Exchange</t>
+  </si>
+  <si>
+    <t>Stack Overflow</t>
+  </si>
+  <si>
+    <t>F47920</t>
+  </si>
+  <si>
+    <t>1F5196</t>
+  </si>
+  <si>
+    <t>2DABE2</t>
   </si>
 </sst>
 </file>
@@ -331,8 +349,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,7 +411,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -410,6 +436,10 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -434,6 +464,10 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,11 +797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -862,94 +896,94 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C5">
-        <v>210.4</v>
+        <v>215</v>
       </c>
       <c r="D5">
         <f>MOD((C5+100),360)</f>
-        <v>310.39999999999998</v>
+        <v>315</v>
       </c>
       <c r="E5">
-        <v>87.3</v>
+        <v>79</v>
       </c>
       <c r="F5">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C6">
-        <v>210</v>
+        <v>210.4</v>
       </c>
       <c r="D6">
         <f>MOD((C6+100),360)</f>
-        <v>310</v>
+        <v>310.39999999999998</v>
       </c>
       <c r="E6">
-        <v>55.1</v>
+        <v>87.3</v>
       </c>
       <c r="F6">
-        <v>38.4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>209.8</v>
+        <v>210</v>
       </c>
       <c r="D7">
         <f>MOD((C7+100),360)</f>
-        <v>309.8</v>
+        <v>310</v>
       </c>
       <c r="E7">
-        <v>66.8</v>
+        <v>55.1</v>
       </c>
       <c r="F7">
-        <v>76.900000000000006</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>207</v>
+        <v>209.8</v>
       </c>
       <c r="D8">
         <f>MOD((C8+100),360)</f>
-        <v>307</v>
+        <v>309.8</v>
       </c>
       <c r="E8">
-        <v>84</v>
+        <v>66.8</v>
       </c>
       <c r="F8">
-        <v>81</v>
+        <v>76.900000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>207</v>
@@ -959,123 +993,123 @@
         <v>307</v>
       </c>
       <c r="E9">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="F9">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D10">
         <f>MOD((C10+100),360)</f>
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="F10">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C11">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D11">
         <f>MOD((C11+100),360)</f>
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E11">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <v>201.8</v>
+        <v>204</v>
       </c>
       <c r="D12">
         <f>MOD((C12+100),360)</f>
-        <v>301.8</v>
+        <v>304</v>
       </c>
       <c r="E12">
-        <v>73.3</v>
+        <v>55</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>199.8</v>
+        <v>201.8</v>
       </c>
       <c r="D13">
         <f>MOD((C13+100),360)</f>
-        <v>299.8</v>
+        <v>301.8</v>
       </c>
       <c r="E13">
-        <v>74.599999999999994</v>
+        <v>73.3</v>
       </c>
       <c r="F13">
-        <v>87.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>199</v>
+        <v>199.8</v>
       </c>
       <c r="D14">
         <f>MOD((C14+100),360)</f>
-        <v>299</v>
+        <v>299.8</v>
       </c>
       <c r="E14">
-        <v>79</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="F14">
-        <v>61</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>199</v>
@@ -1085,259 +1119,259 @@
         <v>299</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F15">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C16">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D16">
         <f>MOD((C16+100),360)</f>
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E16">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F16">
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C17">
-        <v>196.9</v>
+        <v>198</v>
       </c>
       <c r="D17">
         <f>MOD((C17+100),360)</f>
-        <v>296.89999999999998</v>
+        <v>298</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F17">
-        <v>69.400000000000006</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="C18">
-        <v>196.3</v>
+        <v>198</v>
       </c>
       <c r="D18">
         <f>MOD((C18+100),360)</f>
-        <v>296.3</v>
+        <v>298</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F18">
-        <v>94.1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C19">
-        <v>195</v>
+        <v>196.9</v>
       </c>
       <c r="D19">
         <f>MOD((C19+100),360)</f>
-        <v>295</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="E19">
-        <v>4.0999999999999996</v>
+        <v>100</v>
       </c>
       <c r="F19">
-        <v>75.7</v>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>122</v>
+        <v>196.3</v>
       </c>
       <c r="D20">
         <f>MOD((C20+100),360)</f>
-        <v>222</v>
+        <v>296.3</v>
       </c>
       <c r="E20">
-        <v>193</v>
+        <v>100</v>
       </c>
       <c r="F20">
-        <v>66</v>
+        <v>94.1</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C21">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="D21">
         <f>MOD((C21+100),360)</f>
-        <v>184</v>
+        <v>295</v>
       </c>
       <c r="E21">
-        <v>53</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F21">
-        <v>64</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C22">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="D22">
         <f>MOD((C22+100),360)</f>
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="E22">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="F22">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C23">
-        <v>80.900000000000006</v>
+        <v>84</v>
       </c>
       <c r="D23">
         <f>MOD((C23+100),360)</f>
-        <v>180.9</v>
+        <v>184</v>
       </c>
       <c r="E23">
-        <v>86.3</v>
+        <v>53</v>
       </c>
       <c r="F23">
-        <v>71.8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C24">
-        <v>74.5</v>
+        <v>81</v>
       </c>
       <c r="D24">
         <f>MOD((C24+100),360)</f>
-        <v>174.5</v>
+        <v>181</v>
       </c>
       <c r="E24">
-        <v>71.2</v>
+        <v>100</v>
       </c>
       <c r="F24">
-        <v>77.599999999999994</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <v>46</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D25">
         <f>MOD((C25+100),360)</f>
-        <v>146</v>
+        <v>180.9</v>
       </c>
       <c r="E25">
-        <v>59</v>
+        <v>86.3</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C26">
-        <v>42</v>
+        <v>74.5</v>
       </c>
       <c r="D26">
         <f>MOD((C26+100),360)</f>
-        <v>142</v>
+        <v>174.5</v>
       </c>
       <c r="E26">
-        <v>70</v>
+        <v>71.2</v>
       </c>
       <c r="F26">
-        <v>35</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C27">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <f>MOD((C27+100),360)</f>
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F27">
         <v>100</v>
@@ -1345,38 +1379,38 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C28">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <f>MOD((C28+100),360)</f>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <f>MOD((C29+100),360)</f>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E29">
         <v>100</v>
@@ -1387,38 +1421,38 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <f>MOD((C30+100),360)</f>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E30">
         <v>100</v>
       </c>
       <c r="F30">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C31">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D31">
         <f>MOD((C31+100),360)</f>
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -1429,260 +1463,323 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C32">
-        <v>11.2</v>
+        <v>31</v>
       </c>
       <c r="D32">
         <f>MOD((C32+100),360)</f>
-        <v>111.2</v>
+        <v>131</v>
       </c>
       <c r="E32">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F32">
-        <v>92.2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D33">
         <f>MOD((C33+100),360)</f>
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="E33">
-        <v>74.2</v>
+        <v>87</v>
       </c>
       <c r="F33">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D34">
         <f>MOD((C34+100),360)</f>
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="E34">
-        <v>92.5</v>
+        <v>100</v>
       </c>
       <c r="F34">
-        <v>89.4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>11.2</v>
       </c>
       <c r="D35">
         <f>MOD((C35+100),360)</f>
-        <v>103</v>
+        <v>111.2</v>
       </c>
       <c r="E35">
-        <v>97</v>
+        <v>84.7</v>
       </c>
       <c r="F35">
-        <v>84</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <f>MOD((C36+100),360)</f>
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E36">
-        <v>78</v>
+        <v>74.2</v>
       </c>
       <c r="F36">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D37">
         <f>MOD((C37+100),360)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E37">
-        <v>90</v>
+        <v>92.5</v>
       </c>
       <c r="F37">
-        <v>75</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38">
-        <v>444444</v>
+        <v>58</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D38">
         <f>MOD((C38+100),360)</f>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="F38">
-        <v>27</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39">
-        <v>666666</v>
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <f>MOD((C39+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C40">
-        <v>357.5</v>
+        <v>2</v>
       </c>
       <c r="D40">
         <f>MOD((C40+100),360)</f>
-        <v>97.5</v>
+        <v>102</v>
       </c>
       <c r="E40">
-        <v>84.2</v>
+        <v>90</v>
       </c>
       <c r="F40">
-        <v>79.599999999999994</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>444444</v>
       </c>
       <c r="C41">
-        <v>336.8</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <f>MOD((C41+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>100</v>
       </c>
       <c r="E41">
-        <v>67.5</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>91.8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>666666</v>
       </c>
       <c r="C42">
-        <v>328</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <f>MOD((C42+100),360)</f>
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E42">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>93</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C43">
-        <v>287.3</v>
+        <v>357.5</v>
       </c>
       <c r="D43">
         <f>MOD((C43+100),360)</f>
+        <v>97.5</v>
+      </c>
+      <c r="E43">
+        <v>84.2</v>
+      </c>
+      <c r="F43">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>336.8</v>
+      </c>
+      <c r="D44">
+        <f>MOD((C44+100),360)</f>
+        <v>76.800000000000011</v>
+      </c>
+      <c r="E44">
+        <v>67.5</v>
+      </c>
+      <c r="F44">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <v>328</v>
+      </c>
+      <c r="D45">
+        <f>MOD((C45+100),360)</f>
+        <v>68</v>
+      </c>
+      <c r="E45">
+        <v>84</v>
+      </c>
+      <c r="F45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>287.3</v>
+      </c>
+      <c r="D46">
+        <f>MOD((C46+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <v>81.3</v>
       </c>
-      <c r="F43">
+      <c r="F46">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F43">
-      <sortCondition descending="1" ref="D1:D43"/>
+    <sortState ref="A2:F46">
+      <sortCondition descending="1" ref="D1:D46"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Sorting for greys changed.
Suggested by Mendeley’s sysadmin. Good call :-)
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23100" yWindow="1020" windowWidth="9440" windowHeight="18420" tabRatio="500"/>
+    <workbookView xWindow="37360" yWindow="720" windowWidth="11460" windowHeight="26780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,12 +458,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -536,8 +542,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -930,8 +937,8 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -972,7 +979,7 @@
         <v>240</v>
       </c>
       <c r="D2">
-        <f>MOD((C2+100),360)</f>
+        <f t="shared" ref="D2:D33" si="0">MOD((C2+100),360)</f>
         <v>340</v>
       </c>
       <c r="E2">
@@ -993,7 +1000,7 @@
         <v>220.6</v>
       </c>
       <c r="D3">
-        <f>MOD((C3+100),360)</f>
+        <f t="shared" si="0"/>
         <v>320.60000000000002</v>
       </c>
       <c r="E3">
@@ -1014,7 +1021,7 @@
         <v>219</v>
       </c>
       <c r="D4">
-        <f>MOD((C4+100),360)</f>
+        <f t="shared" si="0"/>
         <v>319</v>
       </c>
       <c r="E4">
@@ -1035,7 +1042,7 @@
         <v>217</v>
       </c>
       <c r="D5">
-        <f>MOD((C5+100),360)</f>
+        <f t="shared" si="0"/>
         <v>317</v>
       </c>
       <c r="E5">
@@ -1056,7 +1063,7 @@
         <v>215</v>
       </c>
       <c r="D6">
-        <f>MOD((C6+100),360)</f>
+        <f t="shared" si="0"/>
         <v>315</v>
       </c>
       <c r="E6">
@@ -1077,7 +1084,7 @@
         <v>211</v>
       </c>
       <c r="D7">
-        <f>MOD((C7+100),360)</f>
+        <f t="shared" si="0"/>
         <v>311</v>
       </c>
       <c r="E7">
@@ -1098,7 +1105,7 @@
         <v>210.4</v>
       </c>
       <c r="D8">
-        <f>MOD((C8+100),360)</f>
+        <f t="shared" si="0"/>
         <v>310.39999999999998</v>
       </c>
       <c r="E8">
@@ -1119,7 +1126,7 @@
         <v>210</v>
       </c>
       <c r="D9">
-        <f>MOD((C9+100),360)</f>
+        <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="E9">
@@ -1140,7 +1147,7 @@
         <v>209.8</v>
       </c>
       <c r="D10">
-        <f>MOD((C10+100),360)</f>
+        <f t="shared" si="0"/>
         <v>309.8</v>
       </c>
       <c r="E10">
@@ -1161,7 +1168,7 @@
         <v>207</v>
       </c>
       <c r="D11">
-        <f>MOD((C11+100),360)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E11">
@@ -1182,7 +1189,7 @@
         <v>207</v>
       </c>
       <c r="D12">
-        <f>MOD((C12+100),360)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E12">
@@ -1203,10 +1210,10 @@
         <v>206</v>
       </c>
       <c r="D13">
-        <f>MOD((C13+100),360)</f>
+        <f t="shared" si="0"/>
         <v>306</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>5</v>
       </c>
       <c r="F13">
@@ -1224,7 +1231,7 @@
         <v>205</v>
       </c>
       <c r="D14">
-        <f>MOD((C14+100),360)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="E14">
@@ -1245,7 +1252,7 @@
         <v>202</v>
       </c>
       <c r="D15">
-        <f>MOD((C15+100),360)</f>
+        <f t="shared" si="0"/>
         <v>302</v>
       </c>
       <c r="E15">
@@ -1266,7 +1273,7 @@
         <v>201.8</v>
       </c>
       <c r="D16">
-        <f>MOD((C16+100),360)</f>
+        <f t="shared" si="0"/>
         <v>301.8</v>
       </c>
       <c r="E16">
@@ -1287,7 +1294,7 @@
         <v>200</v>
       </c>
       <c r="D17">
-        <f>MOD((C17+100),360)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="E17">
@@ -1308,7 +1315,7 @@
         <v>199.8</v>
       </c>
       <c r="D18">
-        <f>MOD((C18+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299.8</v>
       </c>
       <c r="E18">
@@ -1329,7 +1336,7 @@
         <v>199</v>
       </c>
       <c r="D19">
-        <f>MOD((C19+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299</v>
       </c>
       <c r="E19">
@@ -1350,7 +1357,7 @@
         <v>199</v>
       </c>
       <c r="D20">
-        <f>MOD((C20+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299</v>
       </c>
       <c r="E20">
@@ -1371,7 +1378,7 @@
         <v>198</v>
       </c>
       <c r="D21">
-        <f>MOD((C21+100),360)</f>
+        <f t="shared" si="0"/>
         <v>298</v>
       </c>
       <c r="E21">
@@ -1392,7 +1399,7 @@
         <v>198</v>
       </c>
       <c r="D22">
-        <f>MOD((C22+100),360)</f>
+        <f t="shared" si="0"/>
         <v>298</v>
       </c>
       <c r="E22">
@@ -1413,7 +1420,7 @@
         <v>196.9</v>
       </c>
       <c r="D23">
-        <f>MOD((C23+100),360)</f>
+        <f t="shared" si="0"/>
         <v>296.89999999999998</v>
       </c>
       <c r="E23">
@@ -1434,7 +1441,7 @@
         <v>196.3</v>
       </c>
       <c r="D24">
-        <f>MOD((C24+100),360)</f>
+        <f t="shared" si="0"/>
         <v>296.3</v>
       </c>
       <c r="E24">
@@ -1455,10 +1462,10 @@
         <v>195</v>
       </c>
       <c r="D25">
-        <f>MOD((C25+100),360)</f>
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="F25">
@@ -1476,7 +1483,7 @@
         <v>194</v>
       </c>
       <c r="D26">
-        <f>MOD((C26+100),360)</f>
+        <f t="shared" si="0"/>
         <v>294</v>
       </c>
       <c r="E26">
@@ -1497,7 +1504,7 @@
         <v>180</v>
       </c>
       <c r="D27">
-        <f>MOD((C27+100),360)</f>
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
       <c r="E27">
@@ -1518,7 +1525,7 @@
         <v>149</v>
       </c>
       <c r="D28">
-        <f>MOD((C28+100),360)</f>
+        <f t="shared" si="0"/>
         <v>249</v>
       </c>
       <c r="E28">
@@ -1539,7 +1546,7 @@
         <v>132</v>
       </c>
       <c r="D29">
-        <f>MOD((C29+100),360)</f>
+        <f t="shared" si="0"/>
         <v>232</v>
       </c>
       <c r="E29">
@@ -1560,7 +1567,7 @@
         <v>122</v>
       </c>
       <c r="D30">
-        <f>MOD((C30+100),360)</f>
+        <f t="shared" si="0"/>
         <v>222</v>
       </c>
       <c r="E30">
@@ -1581,7 +1588,7 @@
         <v>88</v>
       </c>
       <c r="D31">
-        <f>MOD((C31+100),360)</f>
+        <f t="shared" si="0"/>
         <v>188</v>
       </c>
       <c r="E31">
@@ -1602,7 +1609,7 @@
         <v>86</v>
       </c>
       <c r="D32">
-        <f>MOD((C32+100),360)</f>
+        <f t="shared" si="0"/>
         <v>186</v>
       </c>
       <c r="E32">
@@ -1623,7 +1630,7 @@
         <v>84</v>
       </c>
       <c r="D33">
-        <f>MOD((C33+100),360)</f>
+        <f t="shared" si="0"/>
         <v>184</v>
       </c>
       <c r="E33">
@@ -1644,7 +1651,7 @@
         <v>81</v>
       </c>
       <c r="D34">
-        <f>MOD((C34+100),360)</f>
+        <f t="shared" ref="D34:D65" si="1">MOD((C34+100),360)</f>
         <v>181</v>
       </c>
       <c r="E34">
@@ -1665,7 +1672,7 @@
         <v>80.900000000000006</v>
       </c>
       <c r="D35">
-        <f>MOD((C35+100),360)</f>
+        <f t="shared" si="1"/>
         <v>180.9</v>
       </c>
       <c r="E35">
@@ -1686,7 +1693,7 @@
         <v>74.5</v>
       </c>
       <c r="D36">
-        <f>MOD((C36+100),360)</f>
+        <f t="shared" si="1"/>
         <v>174.5</v>
       </c>
       <c r="E36">
@@ -1707,7 +1714,7 @@
         <v>46</v>
       </c>
       <c r="D37">
-        <f>MOD((C37+100),360)</f>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="E37">
@@ -1728,7 +1735,7 @@
         <v>42</v>
       </c>
       <c r="D38">
-        <f>MOD((C38+100),360)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="E38">
@@ -1749,7 +1756,7 @@
         <v>36</v>
       </c>
       <c r="D39">
-        <f>MOD((C39+100),360)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="E39">
@@ -1770,7 +1777,7 @@
         <v>36</v>
       </c>
       <c r="D40">
-        <f>MOD((C40+100),360)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="E40">
@@ -1791,7 +1798,7 @@
         <v>31</v>
       </c>
       <c r="D41">
-        <f>MOD((C41+100),360)</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="E41">
@@ -1812,7 +1819,7 @@
         <v>31</v>
       </c>
       <c r="D42">
-        <f>MOD((C42+100),360)</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="E42">
@@ -1833,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="D43">
-        <f>MOD((C43+100),360)</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="E43">
@@ -1854,7 +1861,7 @@
         <v>25</v>
       </c>
       <c r="D44">
-        <f>MOD((C44+100),360)</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="E44">
@@ -1875,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="D45">
-        <f>MOD((C45+100),360)</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="E45">
@@ -1896,7 +1903,7 @@
         <v>20</v>
       </c>
       <c r="D46">
-        <f>MOD((C46+100),360)</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="E46">
@@ -1917,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="D47">
-        <f>MOD((C47+100),360)</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="E47">
@@ -1938,7 +1945,7 @@
         <v>15</v>
       </c>
       <c r="D48">
-        <f>MOD((C48+100),360)</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="E48">
@@ -1959,7 +1966,7 @@
         <v>12</v>
       </c>
       <c r="D49">
-        <f>MOD((C49+100),360)</f>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="E49">
@@ -1980,7 +1987,7 @@
         <v>11.2</v>
       </c>
       <c r="D50">
-        <f>MOD((C50+100),360)</f>
+        <f t="shared" si="1"/>
         <v>111.2</v>
       </c>
       <c r="E50">
@@ -2001,7 +2008,7 @@
         <v>8</v>
       </c>
       <c r="D51">
-        <f>MOD((C51+100),360)</f>
+        <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="E51">
@@ -2022,7 +2029,7 @@
         <v>7</v>
       </c>
       <c r="D52">
-        <f>MOD((C52+100),360)</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="E52">
@@ -2043,7 +2050,7 @@
         <v>4</v>
       </c>
       <c r="D53">
-        <f>MOD((C53+100),360)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="E53">
@@ -2064,7 +2071,7 @@
         <v>3</v>
       </c>
       <c r="D54">
-        <f>MOD((C54+100),360)</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="E54">
@@ -2085,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <f>MOD((C55+100),360)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="E55">
@@ -2106,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="D56">
-        <f>MOD((C56+100),360)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="E56">
@@ -2127,10 +2134,10 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <f>MOD((C57+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E57" s="1">
         <v>0</v>
       </c>
       <c r="F57">
@@ -2148,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <f>MOD((C58+100),360)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="E58">
@@ -2169,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <f>MOD((C59+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E59" s="1">
         <v>0</v>
       </c>
       <c r="F59">
@@ -2190,10 +2197,10 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <f>MOD((C60+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E60" s="1">
         <v>0</v>
       </c>
       <c r="F60">
@@ -2211,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <f>MOD((C61+100),360)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="E61">
@@ -2232,10 +2239,10 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <f>MOD((C62+100),360)</f>
-        <v>100</v>
-      </c>
-      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E62" s="1">
         <v>0</v>
       </c>
       <c r="F62">
@@ -2253,7 +2260,7 @@
         <v>357.5</v>
       </c>
       <c r="D63">
-        <f>MOD((C63+100),360)</f>
+        <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
       <c r="E63">
@@ -2274,7 +2281,7 @@
         <v>354</v>
       </c>
       <c r="D64">
-        <f>MOD((C64+100),360)</f>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="E64">
@@ -2295,10 +2302,10 @@
         <v>345</v>
       </c>
       <c r="D65">
-        <f>MOD((C65+100),360)</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="1">
         <v>11</v>
       </c>
       <c r="F65">
@@ -2316,7 +2323,7 @@
         <v>336.8</v>
       </c>
       <c r="D66">
-        <f>MOD((C66+100),360)</f>
+        <f t="shared" ref="D66:D97" si="2">MOD((C66+100),360)</f>
         <v>76.800000000000011</v>
       </c>
       <c r="E66">
@@ -2337,7 +2344,7 @@
         <v>328</v>
       </c>
       <c r="D67">
-        <f>MOD((C67+100),360)</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="E67">
@@ -2358,7 +2365,7 @@
         <v>288</v>
       </c>
       <c r="D68">
-        <f>MOD((C68+100),360)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="E68">
@@ -2379,7 +2386,7 @@
         <v>287.3</v>
       </c>
       <c r="D69">
-        <f>MOD((C69+100),360)</f>
+        <f t="shared" si="2"/>
         <v>27.300000000000011</v>
       </c>
       <c r="E69">

</xml_diff>

<commit_message>
Fixed spelling of Codecademy
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -327,9 +327,6 @@
     <t>C68044</t>
   </si>
   <si>
-    <t>Codeacademy</t>
-  </si>
-  <si>
     <t>0088CC</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
   </si>
   <si>
     <t>0066B0</t>
+  </si>
+  <si>
+    <t>Codecademy</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1029,8 @@
   <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1062,16 +1062,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2">
         <v>244</v>
       </c>
       <c r="D2">
-        <f>MOD((C2+100),360)</f>
+        <f t="shared" ref="D2:D33" si="0">MOD((C2+100),360)</f>
         <v>344</v>
       </c>
       <c r="E2">
@@ -1092,7 +1092,7 @@
         <v>240</v>
       </c>
       <c r="D3">
-        <f>MOD((C3+100),360)</f>
+        <f t="shared" si="0"/>
         <v>340</v>
       </c>
       <c r="E3">
@@ -1113,7 +1113,7 @@
         <v>220.6</v>
       </c>
       <c r="D4">
-        <f>MOD((C4+100),360)</f>
+        <f t="shared" si="0"/>
         <v>320.60000000000002</v>
       </c>
       <c r="E4">
@@ -1134,7 +1134,7 @@
         <v>219</v>
       </c>
       <c r="D5">
-        <f>MOD((C5+100),360)</f>
+        <f t="shared" si="0"/>
         <v>319</v>
       </c>
       <c r="E5">
@@ -1146,16 +1146,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
         <v>135</v>
-      </c>
-      <c r="B6" t="s">
-        <v>136</v>
       </c>
       <c r="C6">
         <v>218</v>
       </c>
       <c r="D6">
-        <f>MOD((C6+100),360)</f>
+        <f t="shared" si="0"/>
         <v>318</v>
       </c>
       <c r="E6">
@@ -1167,16 +1167,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
         <v>113</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
       </c>
       <c r="C7">
         <v>217</v>
       </c>
       <c r="D7">
-        <f>MOD((C7+100),360)</f>
+        <f t="shared" si="0"/>
         <v>317</v>
       </c>
       <c r="E7">
@@ -1188,16 +1188,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <v>217</v>
       </c>
       <c r="D8">
-        <f>MOD((C8+100),360)</f>
+        <f t="shared" si="0"/>
         <v>317</v>
       </c>
       <c r="E8">
@@ -1218,7 +1218,7 @@
         <v>215</v>
       </c>
       <c r="D9">
-        <f>MOD((C9+100),360)</f>
+        <f t="shared" si="0"/>
         <v>315</v>
       </c>
       <c r="E9">
@@ -1230,16 +1230,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
         <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
       </c>
       <c r="C10">
         <v>213</v>
       </c>
       <c r="D10">
-        <f>MOD((C10+100),360)</f>
+        <f t="shared" si="0"/>
         <v>313</v>
       </c>
       <c r="E10">
@@ -1251,16 +1251,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
         <v>117</v>
-      </c>
-      <c r="B11" t="s">
-        <v>118</v>
       </c>
       <c r="C11">
         <v>211</v>
       </c>
       <c r="D11">
-        <f>MOD((C11+100),360)</f>
+        <f t="shared" si="0"/>
         <v>311</v>
       </c>
       <c r="E11">
@@ -1281,7 +1281,7 @@
         <v>210.4</v>
       </c>
       <c r="D12">
-        <f>MOD((C12+100),360)</f>
+        <f t="shared" si="0"/>
         <v>310.39999999999998</v>
       </c>
       <c r="E12">
@@ -1302,7 +1302,7 @@
         <v>210</v>
       </c>
       <c r="D13">
-        <f>MOD((C13+100),360)</f>
+        <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="E13">
@@ -1323,7 +1323,7 @@
         <v>209.8</v>
       </c>
       <c r="D14">
-        <f>MOD((C14+100),360)</f>
+        <f t="shared" si="0"/>
         <v>309.8</v>
       </c>
       <c r="E14">
@@ -1344,7 +1344,7 @@
         <v>207</v>
       </c>
       <c r="D15">
-        <f>MOD((C15+100),360)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E15">
@@ -1356,16 +1356,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>137</v>
-      </c>
-      <c r="B16" t="s">
-        <v>138</v>
       </c>
       <c r="C16">
         <v>207</v>
       </c>
       <c r="D16">
-        <f>MOD((C16+100),360)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E16">
@@ -1386,7 +1386,7 @@
         <v>207</v>
       </c>
       <c r="D17">
-        <f>MOD((C17+100),360)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E17">
@@ -1407,7 +1407,7 @@
         <v>206</v>
       </c>
       <c r="D18">
-        <f>MOD((C18+100),360)</f>
+        <f t="shared" si="0"/>
         <v>306</v>
       </c>
       <c r="E18" s="1">
@@ -1419,16 +1419,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19">
         <v>205</v>
       </c>
       <c r="D19">
-        <f>MOD((C19+100),360)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="E19">
@@ -1440,16 +1440,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C20">
         <v>205</v>
       </c>
       <c r="D20">
-        <f>MOD((C20+100),360)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="E20">
@@ -1461,16 +1461,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21">
         <v>205</v>
       </c>
       <c r="D21">
-        <f>MOD((C21+100),360)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="E21">
@@ -1482,16 +1482,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22">
         <v>203</v>
       </c>
       <c r="D22">
-        <f>MOD((C22+100),360)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="E22">
@@ -1503,16 +1503,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23">
         <v>203</v>
       </c>
       <c r="D23">
-        <f>MOD((C23+100),360)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="E23">
@@ -1524,16 +1524,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
         <v>147</v>
-      </c>
-      <c r="B24" t="s">
-        <v>148</v>
       </c>
       <c r="C24">
         <v>203</v>
       </c>
       <c r="D24">
-        <f>MOD((C24+100),360)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="E24">
@@ -1545,16 +1545,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" t="s">
         <v>115</v>
-      </c>
-      <c r="B25" t="s">
-        <v>116</v>
       </c>
       <c r="C25">
         <v>202</v>
       </c>
       <c r="D25">
-        <f>MOD((C25+100),360)</f>
+        <f t="shared" si="0"/>
         <v>302</v>
       </c>
       <c r="E25">
@@ -1575,7 +1575,7 @@
         <v>201.8</v>
       </c>
       <c r="D26">
-        <f>MOD((C26+100),360)</f>
+        <f t="shared" si="0"/>
         <v>301.8</v>
       </c>
       <c r="E26">
@@ -1587,16 +1587,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
         <v>101</v>
-      </c>
-      <c r="B27" t="s">
-        <v>102</v>
       </c>
       <c r="C27">
         <v>200</v>
       </c>
       <c r="D27">
-        <f>MOD((C27+100),360)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="E27">
@@ -1617,7 +1617,7 @@
         <v>199.8</v>
       </c>
       <c r="D28">
-        <f>MOD((C28+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299.8</v>
       </c>
       <c r="E28">
@@ -1638,7 +1638,7 @@
         <v>199</v>
       </c>
       <c r="D29">
-        <f>MOD((C29+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299</v>
       </c>
       <c r="E29">
@@ -1659,7 +1659,7 @@
         <v>199</v>
       </c>
       <c r="D30">
-        <f>MOD((C30+100),360)</f>
+        <f t="shared" si="0"/>
         <v>299</v>
       </c>
       <c r="E30">
@@ -1680,7 +1680,7 @@
         <v>198</v>
       </c>
       <c r="D31">
-        <f>MOD((C31+100),360)</f>
+        <f t="shared" si="0"/>
         <v>298</v>
       </c>
       <c r="E31">
@@ -1701,7 +1701,7 @@
         <v>198</v>
       </c>
       <c r="D32">
-        <f>MOD((C32+100),360)</f>
+        <f t="shared" si="0"/>
         <v>298</v>
       </c>
       <c r="E32">
@@ -1722,7 +1722,7 @@
         <v>196.9</v>
       </c>
       <c r="D33">
-        <f>MOD((C33+100),360)</f>
+        <f t="shared" si="0"/>
         <v>296.89999999999998</v>
       </c>
       <c r="E33">
@@ -1743,7 +1743,7 @@
         <v>196.3</v>
       </c>
       <c r="D34">
-        <f>MOD((C34+100),360)</f>
+        <f t="shared" ref="D34:D65" si="1">MOD((C34+100),360)</f>
         <v>296.3</v>
       </c>
       <c r="E34">
@@ -1764,7 +1764,7 @@
         <v>195</v>
       </c>
       <c r="D35">
-        <f>MOD((C35+100),360)</f>
+        <f t="shared" si="1"/>
         <v>295</v>
       </c>
       <c r="E35" s="1">
@@ -1776,16 +1776,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>194</v>
       </c>
       <c r="D36">
-        <f>MOD((C36+100),360)</f>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
       <c r="E36">
@@ -1806,7 +1806,7 @@
         <v>180</v>
       </c>
       <c r="D37">
-        <f>MOD((C37+100),360)</f>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="E37">
@@ -1827,7 +1827,7 @@
         <v>149</v>
       </c>
       <c r="D38">
-        <f>MOD((C38+100),360)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="E38">
@@ -1839,16 +1839,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39">
         <v>132</v>
       </c>
       <c r="D39">
-        <f>MOD((C39+100),360)</f>
+        <f t="shared" si="1"/>
         <v>232</v>
       </c>
       <c r="E39">
@@ -1869,7 +1869,7 @@
         <v>122</v>
       </c>
       <c r="D40">
-        <f>MOD((C40+100),360)</f>
+        <f t="shared" si="1"/>
         <v>222</v>
       </c>
       <c r="E40">
@@ -1881,16 +1881,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41">
         <v>88</v>
       </c>
       <c r="D41">
-        <f>MOD((C41+100),360)</f>
+        <f t="shared" si="1"/>
         <v>188</v>
       </c>
       <c r="E41">
@@ -1902,16 +1902,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" t="s">
         <v>129</v>
-      </c>
-      <c r="B42" t="s">
-        <v>130</v>
       </c>
       <c r="C42">
         <v>86</v>
       </c>
       <c r="D42">
-        <f>MOD((C42+100),360)</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="E42">
@@ -1932,7 +1932,7 @@
         <v>84</v>
       </c>
       <c r="D43">
-        <f>MOD((C43+100),360)</f>
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="E43">
@@ -1953,7 +1953,7 @@
         <v>81</v>
       </c>
       <c r="D44">
-        <f>MOD((C44+100),360)</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="E44">
@@ -1974,7 +1974,7 @@
         <v>80.900000000000006</v>
       </c>
       <c r="D45">
-        <f>MOD((C45+100),360)</f>
+        <f t="shared" si="1"/>
         <v>180.9</v>
       </c>
       <c r="E45">
@@ -1995,7 +1995,7 @@
         <v>74.5</v>
       </c>
       <c r="D46">
-        <f>MOD((C46+100),360)</f>
+        <f t="shared" si="1"/>
         <v>174.5</v>
       </c>
       <c r="E46">
@@ -2007,16 +2007,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C47">
         <v>51</v>
       </c>
       <c r="D47">
-        <f>MOD((C47+100),360)</f>
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
       <c r="E47">
@@ -2037,7 +2037,7 @@
         <v>46</v>
       </c>
       <c r="D48">
-        <f>MOD((C48+100),360)</f>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="E48">
@@ -2058,7 +2058,7 @@
         <v>42</v>
       </c>
       <c r="D49">
-        <f>MOD((C49+100),360)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="E49">
@@ -2079,7 +2079,7 @@
         <v>36</v>
       </c>
       <c r="D50">
-        <f>MOD((C50+100),360)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="E50">
@@ -2100,7 +2100,7 @@
         <v>36</v>
       </c>
       <c r="D51">
-        <f>MOD((C51+100),360)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="E51">
@@ -2112,16 +2112,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C52">
         <v>36</v>
       </c>
       <c r="D52">
-        <f>MOD((C52+100),360)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="E52">
@@ -2142,7 +2142,7 @@
         <v>31</v>
       </c>
       <c r="D53">
-        <f>MOD((C53+100),360)</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="E53">
@@ -2163,7 +2163,7 @@
         <v>31</v>
       </c>
       <c r="D54">
-        <f>MOD((C54+100),360)</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="E54">
@@ -2184,7 +2184,7 @@
         <v>28</v>
       </c>
       <c r="D55">
-        <f>MOD((C55+100),360)</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="E55">
@@ -2205,7 +2205,7 @@
         <v>25</v>
       </c>
       <c r="D56">
-        <f>MOD((C56+100),360)</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="E56">
@@ -2226,7 +2226,7 @@
         <v>24</v>
       </c>
       <c r="D57">
-        <f>MOD((C57+100),360)</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="E57">
@@ -2238,16 +2238,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
         <v>119</v>
-      </c>
-      <c r="B58" t="s">
-        <v>120</v>
       </c>
       <c r="C58">
         <v>20</v>
       </c>
       <c r="D58">
-        <f>MOD((C58+100),360)</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="E58">
@@ -2259,16 +2259,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C59">
         <v>18</v>
       </c>
       <c r="D59">
-        <f>MOD((C59+100),360)</f>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="E59">
@@ -2280,16 +2280,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
         <v>121</v>
-      </c>
-      <c r="B60" t="s">
-        <v>122</v>
       </c>
       <c r="C60">
         <v>16</v>
       </c>
       <c r="D60">
-        <f>MOD((C60+100),360)</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="E60">
@@ -2301,16 +2301,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" t="s">
         <v>103</v>
-      </c>
-      <c r="B61" t="s">
-        <v>104</v>
       </c>
       <c r="C61">
         <v>15</v>
       </c>
       <c r="D61">
-        <f>MOD((C61+100),360)</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="E61">
@@ -2322,16 +2322,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
         <v>111</v>
-      </c>
-      <c r="B62" t="s">
-        <v>112</v>
       </c>
       <c r="C62">
         <v>12</v>
       </c>
       <c r="D62">
-        <f>MOD((C62+100),360)</f>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="E62">
@@ -2352,7 +2352,7 @@
         <v>11.2</v>
       </c>
       <c r="D63">
-        <f>MOD((C63+100),360)</f>
+        <f t="shared" si="1"/>
         <v>111.2</v>
       </c>
       <c r="E63">
@@ -2364,16 +2364,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" t="s">
         <v>123</v>
-      </c>
-      <c r="B64" t="s">
-        <v>124</v>
       </c>
       <c r="C64">
         <v>8</v>
       </c>
       <c r="D64">
-        <f>MOD((C64+100),360)</f>
+        <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="E64">
@@ -2394,7 +2394,7 @@
         <v>7</v>
       </c>
       <c r="D65">
-        <f>MOD((C65+100),360)</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="E65">
@@ -2415,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="D66">
-        <f>MOD((C66+100),360)</f>
+        <f t="shared" ref="D66:D97" si="2">MOD((C66+100),360)</f>
         <v>104</v>
       </c>
       <c r="E66">
@@ -2436,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="D67">
-        <f>MOD((C67+100),360)</f>
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="E67">
@@ -2457,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <f>MOD((C68+100),360)</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="E68">
@@ -2478,7 +2478,7 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <f>MOD((C69+100),360)</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="E69">
@@ -2490,7 +2490,7 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70">
         <v>870000</v>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f>MOD((C70+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E70">
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f>MOD((C71+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E71">
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f>MOD((C72+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E72" s="1">
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f>MOD((C73+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E73" s="1">
@@ -2574,7 +2574,7 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B74">
         <v>222222</v>
@@ -2583,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f>MOD((C74+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E74" s="1">
@@ -2604,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <f>MOD((C75+100),360)</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E75" s="1">
@@ -2625,7 +2625,7 @@
         <v>357.5</v>
       </c>
       <c r="D76">
-        <f>MOD((C76+100),360)</f>
+        <f t="shared" si="2"/>
         <v>97.5</v>
       </c>
       <c r="E76">
@@ -2637,16 +2637,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
+        <v>132</v>
+      </c>
+      <c r="B77" t="s">
         <v>133</v>
-      </c>
-      <c r="B77" t="s">
-        <v>134</v>
       </c>
       <c r="C77">
         <v>354</v>
       </c>
       <c r="D77">
-        <f>MOD((C77+100),360)</f>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="E77">
@@ -2667,7 +2667,7 @@
         <v>345</v>
       </c>
       <c r="D78">
-        <f>MOD((C78+100),360)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="E78" s="1">
@@ -2688,7 +2688,7 @@
         <v>336.8</v>
       </c>
       <c r="D79">
-        <f>MOD((C79+100),360)</f>
+        <f t="shared" si="2"/>
         <v>76.800000000000011</v>
       </c>
       <c r="E79">
@@ -2700,16 +2700,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C80">
         <v>331</v>
       </c>
       <c r="D80">
-        <f>MOD((C80+100),360)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="E80">
@@ -2730,7 +2730,7 @@
         <v>328</v>
       </c>
       <c r="D81">
-        <f>MOD((C81+100),360)</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="E81">
@@ -2742,16 +2742,16 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C82">
         <v>288</v>
       </c>
       <c r="D82">
-        <f>MOD((C82+100),360)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="E82">
@@ -2772,7 +2772,7 @@
         <v>287.3</v>
       </c>
       <c r="D83">
-        <f>MOD((C83+100),360)</f>
+        <f t="shared" si="2"/>
         <v>27.300000000000011</v>
       </c>
       <c r="E83">

</xml_diff>

<commit_message>
Added Hacker News, JustGiving and Vine
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="1140" windowWidth="12820" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="20580" yWindow="1540" windowWidth="12820" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="184">
   <si>
     <t>Twitter</t>
   </si>
@@ -559,6 +559,21 @@
   </si>
   <si>
     <t>F06529</t>
+  </si>
+  <si>
+    <t>Vine</t>
+  </si>
+  <si>
+    <t>00A47A</t>
+  </si>
+  <si>
+    <t>JustGiving</t>
+  </si>
+  <si>
+    <t>78256D</t>
+  </si>
+  <si>
+    <t>Hacker News</t>
   </si>
 </sst>
 </file>
@@ -613,8 +628,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -732,6 +749,7 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -769,6 +787,7 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1098,11 +1117,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1143,7 +1162,7 @@
         <v>244</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="0">MOD((C2+100),360)</f>
+        <f>MOD((C2+100),360)</f>
         <v>344</v>
       </c>
       <c r="E2">
@@ -1164,7 +1183,7 @@
         <v>240</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>MOD((C3+100),360)</f>
         <v>340</v>
       </c>
       <c r="E3">
@@ -1185,7 +1204,7 @@
         <v>220.6</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>MOD((C4+100),360)</f>
         <v>320.60000000000002</v>
       </c>
       <c r="E4">
@@ -1206,7 +1225,7 @@
         <v>219</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>MOD((C5+100),360)</f>
         <v>319</v>
       </c>
       <c r="E5">
@@ -1227,7 +1246,7 @@
         <v>218</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>MOD((C6+100),360)</f>
         <v>318</v>
       </c>
       <c r="E6">
@@ -1248,7 +1267,7 @@
         <v>217</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>MOD((C7+100),360)</f>
         <v>317</v>
       </c>
       <c r="E7">
@@ -1269,7 +1288,7 @@
         <v>217</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>MOD((C8+100),360)</f>
         <v>317</v>
       </c>
       <c r="E8">
@@ -1290,7 +1309,7 @@
         <v>215</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>MOD((C9+100),360)</f>
         <v>315</v>
       </c>
       <c r="E9">
@@ -1311,7 +1330,7 @@
         <v>213</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>MOD((C10+100),360)</f>
         <v>313</v>
       </c>
       <c r="E10">
@@ -1332,7 +1351,7 @@
         <v>211</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>MOD((C11+100),360)</f>
         <v>311</v>
       </c>
       <c r="E11">
@@ -1353,7 +1372,7 @@
         <v>210.4</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f>MOD((C12+100),360)</f>
         <v>310.39999999999998</v>
       </c>
       <c r="E12">
@@ -1374,7 +1393,7 @@
         <v>210</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>MOD((C13+100),360)</f>
         <v>310</v>
       </c>
       <c r="E13">
@@ -1395,7 +1414,7 @@
         <v>209.8</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>MOD((C14+100),360)</f>
         <v>309.8</v>
       </c>
       <c r="E14">
@@ -1416,7 +1435,7 @@
         <v>208</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>MOD((C15+100),360)</f>
         <v>308</v>
       </c>
       <c r="E15">
@@ -1437,7 +1456,7 @@
         <v>207</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>MOD((C16+100),360)</f>
         <v>307</v>
       </c>
       <c r="E16">
@@ -1458,7 +1477,7 @@
         <v>207</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f>MOD((C17+100),360)</f>
         <v>307</v>
       </c>
       <c r="E17">
@@ -1479,7 +1498,7 @@
         <v>207</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>MOD((C18+100),360)</f>
         <v>307</v>
       </c>
       <c r="E18">
@@ -1500,7 +1519,7 @@
         <v>206</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>MOD((C19+100),360)</f>
         <v>306</v>
       </c>
       <c r="E19" s="1">
@@ -1521,7 +1540,7 @@
         <v>205</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f>MOD((C20+100),360)</f>
         <v>305</v>
       </c>
       <c r="E20">
@@ -1542,7 +1561,7 @@
         <v>205</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>MOD((C21+100),360)</f>
         <v>305</v>
       </c>
       <c r="E21">
@@ -1563,7 +1582,7 @@
         <v>205</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>MOD((C22+100),360)</f>
         <v>305</v>
       </c>
       <c r="E22">
@@ -1584,7 +1603,7 @@
         <v>204</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>MOD((C23+100),360)</f>
         <v>304</v>
       </c>
       <c r="E23">
@@ -1605,7 +1624,7 @@
         <v>203</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>MOD((C24+100),360)</f>
         <v>303</v>
       </c>
       <c r="E24">
@@ -1626,7 +1645,7 @@
         <v>203</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>MOD((C25+100),360)</f>
         <v>303</v>
       </c>
       <c r="E25">
@@ -1647,7 +1666,7 @@
         <v>203</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f>MOD((C26+100),360)</f>
         <v>303</v>
       </c>
       <c r="E26">
@@ -1668,7 +1687,7 @@
         <v>202</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f>MOD((C27+100),360)</f>
         <v>302</v>
       </c>
       <c r="E27">
@@ -1689,7 +1708,7 @@
         <v>201.8</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>MOD((C28+100),360)</f>
         <v>301.8</v>
       </c>
       <c r="E28">
@@ -1710,7 +1729,7 @@
         <v>200</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>MOD((C29+100),360)</f>
         <v>300</v>
       </c>
       <c r="E29">
@@ -1731,7 +1750,7 @@
         <v>199.8</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>MOD((C30+100),360)</f>
         <v>299.8</v>
       </c>
       <c r="E30">
@@ -1752,7 +1771,7 @@
         <v>199</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f>MOD((C31+100),360)</f>
         <v>299</v>
       </c>
       <c r="E31">
@@ -1773,7 +1792,7 @@
         <v>199</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f>MOD((C32+100),360)</f>
         <v>299</v>
       </c>
       <c r="E32">
@@ -1794,7 +1813,7 @@
         <v>198</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f>MOD((C33+100),360)</f>
         <v>298</v>
       </c>
       <c r="E33">
@@ -1815,7 +1834,7 @@
         <v>198</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="1">MOD((C34+100),360)</f>
+        <f>MOD((C34+100),360)</f>
         <v>298</v>
       </c>
       <c r="E34">
@@ -1836,7 +1855,7 @@
         <v>196.9</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f>MOD((C35+100),360)</f>
         <v>296.89999999999998</v>
       </c>
       <c r="E35">
@@ -1857,7 +1876,7 @@
         <v>196.3</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f>MOD((C36+100),360)</f>
         <v>296.3</v>
       </c>
       <c r="E36">
@@ -1878,7 +1897,7 @@
         <v>195</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f>MOD((C37+100),360)</f>
         <v>295</v>
       </c>
       <c r="E37" s="1">
@@ -1899,7 +1918,7 @@
         <v>194</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f>MOD((C38+100),360)</f>
         <v>294</v>
       </c>
       <c r="E38">
@@ -1920,7 +1939,7 @@
         <v>194</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f>MOD((C39+100),360)</f>
         <v>294</v>
       </c>
       <c r="E39">
@@ -1941,7 +1960,7 @@
         <v>180</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f>MOD((C40+100),360)</f>
         <v>280</v>
       </c>
       <c r="E40">
@@ -1953,146 +1972,146 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="C41">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
-        <v>249</v>
+        <f>MOD((C41+100),360)</f>
+        <v>265</v>
       </c>
       <c r="E41">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F41">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C42">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
-        <v>232</v>
+        <f>MOD((C42+100),360)</f>
+        <v>249</v>
       </c>
       <c r="E42">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="F42">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="C43">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
-        <v>222</v>
+        <f>MOD((C43+100),360)</f>
+        <v>232</v>
       </c>
       <c r="E43">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F43">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="C44">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
-        <v>188</v>
+        <f>MOD((C44+100),360)</f>
+        <v>222</v>
       </c>
       <c r="E44">
+        <v>193</v>
+      </c>
+      <c r="F44">
         <v>66</v>
-      </c>
-      <c r="F44">
-        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
-        <v>186</v>
+        <f>MOD((C45+100),360)</f>
+        <v>188</v>
       </c>
       <c r="E45">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F45">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="C46">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
-        <v>184</v>
+        <f>MOD((C46+100),360)</f>
+        <v>186</v>
       </c>
       <c r="E46">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="F46">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C47">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
-        <v>181</v>
+        <f>MOD((C47+100),360)</f>
+        <v>184</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="F47">
         <v>64</v>
@@ -2100,154 +2119,154 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C48">
-        <v>80.900000000000006</v>
+        <v>81</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
-        <v>180.9</v>
+        <f>MOD((C48+100),360)</f>
+        <v>181</v>
       </c>
       <c r="E48">
-        <v>86.3</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>71.8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C49">
-        <v>74.5</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
-        <v>174.5</v>
+        <f>MOD((C49+100),360)</f>
+        <v>180.9</v>
       </c>
       <c r="E49">
-        <v>71.2</v>
+        <v>86.3</v>
       </c>
       <c r="F49">
-        <v>77.599999999999994</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>38</v>
       </c>
       <c r="C50">
-        <v>51</v>
+        <v>74.5</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
-        <v>151</v>
+        <f>MOD((C50+100),360)</f>
+        <v>174.5</v>
       </c>
       <c r="E50">
-        <v>100</v>
+        <v>71.2</v>
       </c>
       <c r="F50">
-        <v>95</v>
+        <v>77.599999999999994</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="C51">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
-        <v>146</v>
+        <f>MOD((C51+100),360)</f>
+        <v>151</v>
       </c>
       <c r="E51">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F51">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C52">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
-        <v>142</v>
+        <f>MOD((C52+100),360)</f>
+        <v>146</v>
       </c>
       <c r="E52">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F52">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="C53">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
-        <v>138</v>
+        <f>MOD((C53+100),360)</f>
+        <v>142</v>
       </c>
       <c r="E53">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F53">
-        <v>97</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="C54">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
-        <v>136</v>
+        <f>MOD((C54+100),360)</f>
+        <v>138</v>
       </c>
       <c r="E54">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F54">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
@@ -2256,7 +2275,7 @@
         <v>36</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
+        <f>MOD((C55+100),360)</f>
         <v>136</v>
       </c>
       <c r="E55">
@@ -2268,7 +2287,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -2277,7 +2296,7 @@
         <v>36</v>
       </c>
       <c r="D56">
-        <f t="shared" si="1"/>
+        <f>MOD((C56+100),360)</f>
         <v>136</v>
       </c>
       <c r="E56">
@@ -2289,20 +2308,20 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="C57">
         <v>36</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
+        <f>MOD((C57+100),360)</f>
         <v>136</v>
       </c>
       <c r="E57">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F57">
         <v>100</v>
@@ -2310,20 +2329,20 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C58">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
-        <v>131</v>
+        <f>MOD((C58+100),360)</f>
+        <v>136</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F58">
         <v>100</v>
@@ -2331,722 +2350,785 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C59">
         <v>31</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
+        <f>MOD((C59+100),360)</f>
         <v>131</v>
       </c>
       <c r="E59">
         <v>100</v>
       </c>
       <c r="F59">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C60">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
-        <v>128</v>
+        <f>MOD((C60+100),360)</f>
+        <v>131</v>
       </c>
       <c r="E60">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="F60">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C61">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D61">
-        <f t="shared" si="1"/>
-        <v>125</v>
+        <f>MOD((C61+100),360)</f>
+        <v>128</v>
       </c>
       <c r="E61">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F61">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="C62">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D62">
-        <f t="shared" si="1"/>
-        <v>124</v>
+        <f>MOD((C62+100),360)</f>
+        <v>125</v>
       </c>
       <c r="E62">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F62">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="C63">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D63">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>MOD((C63+100),360)</f>
+        <v>124</v>
       </c>
       <c r="E63">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="F63">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="C64">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D64">
-        <f t="shared" si="1"/>
-        <v>118</v>
+        <f>MOD((C64+100),360)</f>
+        <v>124</v>
       </c>
       <c r="E64">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F64">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <f>MOD((C65+100),360)</f>
         <v>120</v>
       </c>
-      <c r="B65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C65">
-        <v>16</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
       <c r="E65">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="F65">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="C66">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D97" si="2">MOD((C66+100),360)</f>
-        <v>115</v>
+        <f>MOD((C66+100),360)</f>
+        <v>118</v>
       </c>
       <c r="E66">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F66">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C67">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D67">
-        <f t="shared" si="2"/>
-        <v>112</v>
+        <f>MOD((C67+100),360)</f>
+        <v>116</v>
       </c>
       <c r="E67">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F67">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="C68">
-        <v>11.2</v>
+        <v>15</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
-        <v>111.2</v>
+        <f>MOD((C68+100),360)</f>
+        <v>115</v>
       </c>
       <c r="E68">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F68">
-        <v>92.2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
-        <v>108</v>
+        <f>MOD((C69+100),360)</f>
+        <v>112</v>
       </c>
       <c r="E69">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F69">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C70">
-        <v>7</v>
+        <v>11.2</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
-        <v>107</v>
+        <f>MOD((C70+100),360)</f>
+        <v>111.2</v>
       </c>
       <c r="E70">
-        <v>74.2</v>
+        <v>84.7</v>
       </c>
       <c r="F70">
-        <v>82</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
-        <v>104</v>
+        <f>MOD((C71+100),360)</f>
+        <v>108</v>
       </c>
       <c r="E71">
-        <v>92.5</v>
+        <v>81</v>
       </c>
       <c r="F71">
-        <v>89.4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
-        <v>103</v>
+        <f>MOD((C72+100),360)</f>
+        <v>107</v>
       </c>
       <c r="E72">
-        <v>97</v>
+        <v>74.2</v>
       </c>
       <c r="F72">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D73">
-        <f t="shared" si="2"/>
-        <v>102</v>
+        <f>MOD((C73+100),360)</f>
+        <v>104</v>
       </c>
       <c r="E73">
-        <v>78</v>
+        <v>92.5</v>
       </c>
       <c r="F73">
-        <v>80</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <f>MOD((C74+100),360)</f>
+        <v>103</v>
+      </c>
+      <c r="E74">
+        <v>97</v>
+      </c>
+      <c r="F74">
         <v>84</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
-      </c>
-      <c r="D74">
-        <f t="shared" si="2"/>
-        <v>102</v>
-      </c>
-      <c r="E74">
-        <v>90</v>
-      </c>
-      <c r="F74">
-        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f>MOD((C75+100),360)</f>
+        <v>102</v>
       </c>
       <c r="E75">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F75">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f>MOD((C76+100),360)</f>
+        <v>102</v>
       </c>
       <c r="E76">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F76">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>125</v>
-      </c>
-      <c r="B77">
-        <v>870000</v>
+        <v>168</v>
+      </c>
+      <c r="B77" t="s">
+        <v>174</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f>MOD((C77+100),360)</f>
         <v>100</v>
       </c>
       <c r="E77">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F77">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>62</v>
-      </c>
-      <c r="B78">
-        <v>666666</v>
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
+        <v>96</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="E78" s="1">
-        <v>0</v>
+        <f>MOD((C78+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>93</v>
       </c>
       <c r="F78">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="B79">
-        <v>444444</v>
+        <v>870000</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="E79" s="1">
-        <v>0</v>
+        <f>MOD((C79+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>100</v>
       </c>
       <c r="F79">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="B80">
-        <v>222222</v>
+        <v>666666</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <f t="shared" si="2"/>
+        <f>MOD((C80+100),360)</f>
         <v>100</v>
       </c>
       <c r="E80" s="1">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>444444</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f>MOD((C81+100),360)</f>
         <v>100</v>
       </c>
       <c r="E81" s="1">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>222222</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f>MOD((C82+100),360)</f>
         <v>100</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>8</v>
-      </c>
-      <c r="B83" t="s">
-        <v>16</v>
+        <v>93</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
-        <v>97.5</v>
-      </c>
-      <c r="E83">
-        <v>84.2</v>
+        <f>MOD((C83+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>79.599999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>132</v>
-      </c>
-      <c r="B84" t="s">
-        <v>133</v>
+        <v>167</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
-        <v>94</v>
-      </c>
-      <c r="E84">
-        <v>83</v>
+        <f>MOD((C84+100),360)</f>
+        <v>100</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="C85">
-        <v>350</v>
+        <v>357.5</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
-        <v>90</v>
+        <f>MOD((C85+100),360)</f>
+        <v>97.5</v>
       </c>
       <c r="E85">
-        <v>91</v>
+        <v>84.2</v>
       </c>
       <c r="F85">
-        <v>77</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C86">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="E86" s="1">
-        <v>11</v>
+        <f>MOD((C86+100),360)</f>
+        <v>94</v>
+      </c>
+      <c r="E86">
+        <v>83</v>
       </c>
       <c r="F86">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="C87">
-        <v>336.8</v>
+        <v>350</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
-        <v>76.800000000000011</v>
+        <f>MOD((C87+100),360)</f>
+        <v>90</v>
       </c>
       <c r="E87">
-        <v>67.5</v>
+        <v>91</v>
       </c>
       <c r="F87">
-        <v>91.8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="C88">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-      <c r="E88">
-        <v>88</v>
+        <f>MOD((C88+100),360)</f>
+        <v>85</v>
+      </c>
+      <c r="E88" s="1">
+        <v>11</v>
       </c>
       <c r="F88">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C89">
-        <v>328</v>
+        <v>336.8</v>
       </c>
       <c r="D89">
-        <f t="shared" si="2"/>
-        <v>68</v>
+        <f>MOD((C89+100),360)</f>
+        <v>76.800000000000011</v>
       </c>
       <c r="E89">
-        <v>84</v>
+        <v>67.5</v>
       </c>
       <c r="F89">
-        <v>93</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C90">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="D90">
-        <f t="shared" si="2"/>
-        <v>62</v>
+        <f>MOD((C90+100),360)</f>
+        <v>71</v>
       </c>
       <c r="E90">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F90">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="C91">
-        <v>288</v>
+        <v>328</v>
       </c>
       <c r="D91">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f>MOD((C91+100),360)</f>
+        <v>68</v>
       </c>
       <c r="E91">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F91">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
+        <v>166</v>
+      </c>
+      <c r="B92" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92">
+        <v>322</v>
+      </c>
+      <c r="D92">
+        <f>MOD((C92+100),360)</f>
+        <v>62</v>
+      </c>
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="F92">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93">
+        <v>308</v>
+      </c>
+      <c r="D93">
+        <f>MOD((C93+100),360)</f>
+        <v>48</v>
+      </c>
+      <c r="E93">
+        <v>69</v>
+      </c>
+      <c r="F93">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94">
+        <v>288</v>
+      </c>
+      <c r="D94">
+        <f>MOD((C94+100),360)</f>
+        <v>28</v>
+      </c>
+      <c r="E94">
+        <v>73</v>
+      </c>
+      <c r="F94">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
         <v>33</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B95" t="s">
         <v>34</v>
       </c>
-      <c r="C92">
+      <c r="C95">
         <v>287.3</v>
       </c>
-      <c r="D92">
-        <f t="shared" si="2"/>
+      <c r="D95">
+        <f>MOD((C95+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E92">
+      <c r="E95">
         <v>81.3</v>
       </c>
-      <c r="F92">
+      <c r="F95">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F92">
-      <sortCondition descending="1" ref="D1:D92"/>
+    <sortState ref="A2:F95">
+      <sortCondition descending="1" ref="D1:D95"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Laravel and TED
</commit_message>
<xml_diff>
--- a/Sortable Colour Data.xlsx
+++ b/Sortable Colour Data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="188">
   <si>
     <t>Twitter</t>
   </si>
@@ -574,6 +574,18 @@
   </si>
   <si>
     <t>Hacker News</t>
+  </si>
+  <si>
+    <t>TED</t>
+  </si>
+  <si>
+    <t>FF2B06</t>
+  </si>
+  <si>
+    <t>Laravel</t>
+  </si>
+  <si>
+    <t>FB502B</t>
   </si>
 </sst>
 </file>
@@ -1117,11 +1129,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2602,178 +2614,178 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="B71" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D71">
         <f>MOD((C71+100),360)</f>
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E71">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F71">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="C72">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <f>MOD((C72+100),360)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E72">
-        <v>74.2</v>
+        <v>81</v>
       </c>
       <c r="F72">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" t="s">
+        <v>187</v>
+      </c>
+      <c r="C73">
         <v>7</v>
-      </c>
-      <c r="B73" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73">
-        <v>4</v>
       </c>
       <c r="D73">
         <f>MOD((C73+100),360)</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E73">
-        <v>92.5</v>
+        <v>76</v>
       </c>
       <c r="F73">
-        <v>89.4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D74">
         <f>MOD((C74+100),360)</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E74">
-        <v>97</v>
+        <v>74.2</v>
       </c>
       <c r="F74">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D75">
         <f>MOD((C75+100),360)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E75">
-        <v>78</v>
+        <v>92.5</v>
       </c>
       <c r="F75">
-        <v>80</v>
+        <v>89.4</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D76">
         <f>MOD((C76+100),360)</f>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E76">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F76">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D77">
         <f>MOD((C77+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E77">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F77">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D78">
         <f>MOD((C78+100),360)</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E78">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F78">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79">
-        <v>870000</v>
+        <v>168</v>
+      </c>
+      <c r="B79" t="s">
+        <v>174</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2783,18 +2795,18 @@
         <v>100</v>
       </c>
       <c r="E79">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F79">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>62</v>
-      </c>
-      <c r="B80">
-        <v>666666</v>
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
+        <v>96</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2803,19 +2815,19 @@
         <f>MOD((C80+100),360)</f>
         <v>100</v>
       </c>
-      <c r="E80" s="1">
-        <v>0</v>
+      <c r="E80">
+        <v>93</v>
       </c>
       <c r="F80">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="B81">
-        <v>444444</v>
+        <v>870000</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2824,19 +2836,19 @@
         <f>MOD((C81+100),360)</f>
         <v>100</v>
       </c>
-      <c r="E81" s="1">
-        <v>0</v>
+      <c r="E81">
+        <v>100</v>
       </c>
       <c r="F81">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="B82">
-        <v>222222</v>
+        <v>666666</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2849,15 +2861,15 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>444444</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2870,15 +2882,15 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>222222</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2891,244 +2903,286 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" t="s">
-        <v>16</v>
+        <v>93</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>357.5</v>
+        <v>0</v>
       </c>
       <c r="D85">
         <f>MOD((C85+100),360)</f>
-        <v>97.5</v>
-      </c>
-      <c r="E85">
-        <v>84.2</v>
+        <v>100</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>79.599999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" t="s">
-        <v>133</v>
+        <v>167</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <f>MOD((C86+100),360)</f>
-        <v>94</v>
-      </c>
-      <c r="E86">
-        <v>83</v>
+        <v>100</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="C87">
-        <v>350</v>
+        <v>357.5</v>
       </c>
       <c r="D87">
         <f>MOD((C87+100),360)</f>
-        <v>90</v>
+        <v>97.5</v>
       </c>
       <c r="E87">
-        <v>91</v>
+        <v>84.2</v>
       </c>
       <c r="F87">
-        <v>77</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C88">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="D88">
         <f>MOD((C88+100),360)</f>
-        <v>85</v>
-      </c>
-      <c r="E88" s="1">
-        <v>11</v>
+        <v>94</v>
+      </c>
+      <c r="E88">
+        <v>83</v>
       </c>
       <c r="F88">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="C89">
-        <v>336.8</v>
+        <v>350</v>
       </c>
       <c r="D89">
         <f>MOD((C89+100),360)</f>
-        <v>76.800000000000011</v>
+        <v>90</v>
       </c>
       <c r="E89">
-        <v>67.5</v>
+        <v>91</v>
       </c>
       <c r="F89">
-        <v>91.8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="B90" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="C90">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="D90">
         <f>MOD((C90+100),360)</f>
-        <v>71</v>
-      </c>
-      <c r="E90">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="E90" s="1">
+        <v>11</v>
       </c>
       <c r="F90">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C91">
-        <v>328</v>
+        <v>336.8</v>
       </c>
       <c r="D91">
         <f>MOD((C91+100),360)</f>
-        <v>68</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="E91">
-        <v>84</v>
+        <v>67.5</v>
       </c>
       <c r="F91">
-        <v>93</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C92">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="D92">
         <f>MOD((C92+100),360)</f>
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E92">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F92">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>67</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>71</v>
       </c>
       <c r="C93">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="D93">
         <f>MOD((C93+100),360)</f>
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E93">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F93">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="C94">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="D94">
         <f>MOD((C94+100),360)</f>
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="E94">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="F94">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="B95" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="C95">
-        <v>287.3</v>
+        <v>308</v>
       </c>
       <c r="D95">
         <f>MOD((C95+100),360)</f>
+        <v>48</v>
+      </c>
+      <c r="E95">
+        <v>69</v>
+      </c>
+      <c r="F95">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C96">
+        <v>288</v>
+      </c>
+      <c r="D96">
+        <f>MOD((C96+100),360)</f>
+        <v>28</v>
+      </c>
+      <c r="E96">
+        <v>73</v>
+      </c>
+      <c r="F96">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97">
+        <v>287.3</v>
+      </c>
+      <c r="D97">
+        <f>MOD((C97+100),360)</f>
         <v>27.300000000000011</v>
       </c>
-      <c r="E95">
+      <c r="E97">
         <v>81.3</v>
       </c>
-      <c r="F95">
+      <c r="F97">
         <v>54.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
-    <sortState ref="A2:F95">
-      <sortCondition descending="1" ref="D1:D95"/>
+    <sortState ref="A2:F97">
+      <sortCondition descending="1" ref="D1:D97"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>